<commit_message>
feat: Initial stable release of M3X bridge
First stable release containing all necessary files for hardware replication and firmware installation. Files included: * Firmware/01_Web_Touch_Console/M3X_Web_Control_v1.0.bin (Pre-compiled firmware) * Docs/BOM_v1.0.xlsx & Docs/ESP32_C3_Core_Introduction.md * Docs/Flashing_Guide.md (Instructions for burning the BIN file) * Hardware/PCB_Gerber/Gerber_M3X_Rev1_0.zip (For PCB manufacturing) * Hardware/Case_Drawings/1152(3-59-2).dwg & .pdf (2D case drawings)
</commit_message>
<xml_diff>
--- a/Docs/BOM_v1.0.xlsx
+++ b/Docs/BOM_v1.0.xlsx
@@ -1,10 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29426"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DD088E2-22AC-41B4-8BE2-4D5F8571530C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet sheetId="1" name="BOM_Board1_M3W_2025-12-12" state="visible" r:id="rId4"/>
+    <sheet name="BOM_Board1_M3W_2025-12-12" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
@@ -178,32 +182,40 @@
     <t>U1</t>
   </si>
   <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>MAX232ACSE</t>
+  </si>
+  <si>
+    <t>U4</t>
+  </si>
+  <si>
+    <t>SOP-16_L10.0-W3.9-P1.27-LS6.0-BL</t>
+  </si>
+  <si>
     <t>ESP32_C3_mini</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>MAX232ACSE</t>
-  </si>
-  <si>
-    <t>U4</t>
-  </si>
-  <si>
-    <t>SOP-16_L10.0-W3.9-P1.27-LS6.0-BL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -230,7 +242,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -566,14 +578,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="10" width="20" customWidth="1"/>
+    <col min="1" max="4" width="20" customWidth="1"/>
+    <col min="5" max="5" width="23.1796875" customWidth="1"/>
+    <col min="6" max="10" width="20" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -814,7 +830,7 @@
         <v>54</v>
       </c>
       <c r="E8" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="F8" t="s">
         <v>36</v>
@@ -834,20 +850,20 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
       <c r="C9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" t="s">
         <v>57</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>58</v>
       </c>
-      <c r="E9" t="s">
-        <v>59</v>
-      </c>
       <c r="F9" t="s">
         <v>36</v>
       </c>
@@ -864,14 +880,15 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>36</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
</xml_diff>